<commit_message>
removed test trial test output files and added new test class
</commit_message>
<xml_diff>
--- a/src/test/java/utility/TestData.xlsx
+++ b/src/test/java/utility/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14925" windowHeight="4215"/>
   </bookViews>
   <sheets>
     <sheet name="TopRatedMovies" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>poster_path</t>
   </si>
@@ -24,19 +25,10 @@
     <t>adult</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>overview</t>
   </si>
   <si>
-    <t xml:space="preserve">string </t>
-  </si>
-  <si>
     <t>Results</t>
-  </si>
-  <si>
-    <t>array</t>
   </si>
 </sst>
 </file>
@@ -72,11 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,48 +360,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>